<commit_message>
6 10K RES wrong component 5.1Ω
</commit_message>
<xml_diff>
--- a/production/v1.1/S2-BOM.xlsx
+++ b/production/v1.1/S2-BOM.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
   <si>
     <t>R_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>SOT-23</t>
   </si>
   <si>
     <t>LED_0805_2012Metric</t>
@@ -49,9 +46,6 @@
   </si>
   <si>
     <t>ESP32-S2-WROVER</t>
-  </si>
-  <si>
-    <t>C92959</t>
   </si>
 </sst>
 </file>
@@ -100,11 +94,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
+  <cellXfs count="1">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
@@ -121,7 +111,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.45"/>
@@ -130,7 +120,7 @@
     <col min="2" max="2" style="0" width="21.998677884615386" customWidth="1"/>
     <col min="3" max="3" style="0" width="32.855168269230774" customWidth="1"/>
     <col min="4" max="4" style="0" width="44.14972756410257" customWidth="1"/>
-    <col min="5" max="256" style="0" width="9.142307692307693"/>
+    <col min="5" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.5">
@@ -149,7 +139,7 @@
           <t>Comment</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>JLCPCB Part #</t>
         </is>
@@ -171,7 +161,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C25197</t>
+          <t>C25804</t>
         </is>
       </c>
     </row>
@@ -181,8 +171,10 @@
           <t>Q2,Q1</t>
         </is>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -246,7 +238,7 @@
         </is>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -266,7 +258,7 @@
         </is>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -306,7 +298,7 @@
         </is>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -326,15 +318,15 @@
         </is>
       </c>
       <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BOOT</t>
+        </is>
+      </c>
+      <c r="D10" t="s">
         <v>4</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BOOT</t>
-        </is>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.5">
@@ -364,7 +356,7 @@
         </is>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -406,7 +398,7 @@
         </is>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -434,7 +426,7 @@
         </is>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5">
@@ -444,7 +436,7 @@
         </is>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -452,7 +444,7 @@
         </is>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.5">
@@ -470,7 +462,7 @@
         </is>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5">
@@ -538,7 +530,7 @@
         </is>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -558,7 +550,7 @@
         </is>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -586,7 +578,7 @@
         </is>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5">
@@ -626,7 +618,7 @@
         </is>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5">
@@ -658,7 +650,7 @@
         </is>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -666,7 +658,7 @@
         </is>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5">
@@ -696,10 +688,10 @@
         </is>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -734,7 +726,7 @@
         </is>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -776,15 +768,15 @@
         </is>
       </c>
       <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>RESET</t>
+        </is>
+      </c>
+      <c r="D33" t="s">
         <v>4</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>RESET</t>
-        </is>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13.5">
@@ -825,8 +817,10 @@
           <t>2.2uH</t>
         </is>
       </c>
-      <c r="D35" t="s">
-        <v>10</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>C92959</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>